<commit_message>
created pipeline stage register
</commit_message>
<xml_diff>
--- a/control_signal_per_pipe_stage.xlsx
+++ b/control_signal_per_pipe_stage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPRE381Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FFF6BE-599E-4D05-A698-BFDD22C6C5FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565612F3-F460-411E-956D-2466B5333A86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46516AFA-8383-4921-9F79-CAEC1EFA5A83}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{46516AFA-8383-4921-9F79-CAEC1EFA5A83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A061969-741A-4F63-9A1C-5AF1F1190A44}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="152" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="152" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>